<commit_message>
Fleshed out elections spreadsheet
</commit_message>
<xml_diff>
--- a/data/Elections by State.xlsx
+++ b/data/Elections by State.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A40102C-4C43-A147-B289-7445B8AC09CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3745F743-3855-4C4A-A7C3-ADAF7DCA185C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="3420" windowWidth="27260" windowHeight="16940" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
+    <workbookView xWindow="13940" yWindow="3420" windowWidth="27260" windowHeight="16940" activeTab="1" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Elections by State" sheetId="2" r:id="rId1"/>
+    <sheet name="Criteria" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Elections by State'!$E$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Elections by State'!$E$1:$L$51</definedName>
     <definedName name="elections_1" localSheetId="0">'Elections by State'!$A$3:$T$50</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="196">
   <si>
     <t>AL</t>
   </si>
@@ -507,6 +508,156 @@
   </si>
   <si>
     <t>MAP</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/969193c5-8e5a-4bb6-b587-9ba7133fadfd</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/b2688b81-4db7-4739-aa51-8629e7bd6266</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/7b49059d-9e45-4de6-bbf8-fe6992829412</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/ea1c72c0-0074-42fb-a991-13b78672a6e6</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/18cac456-364a-4181-8fb9-c1a63bc99d1d</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/360e7912-f54c-4e67-b284-05540af56c6a</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/d7fe5e94-48f3-4224-b5a8-04ce33550aa4</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/ae4ffddf-50d7-49df-ab73-fa74292ccc38</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/31732abd-960b-4fe7-8c67-62dc85c7e236</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/1e3875e9-0906-442e-aa75-a963673a62ca</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/e20e9219-de74-4b66-96d4-5d3fd3c36cfc</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/f1aa40ba-3a37-4b87-9ce1-b8d64caa64a6</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/0a41162a-6ff1-4ae2-aeb6-14c6ab4e8cdb</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/85a2710a-3d94-4ea5-81de-ccf6f11d9a77</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/82731456-645b-47b8-9d7e-61bb73e65e51</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/8cede98f-f2f7-4812-8d0e-c596d2ae5838</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/06bbc006-e00c-4e3e-a386-0942f515704c</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/9aebf80b-5d84-491c-ba52-f64d31697cb2</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/92f30641-08af-423e-a7dd-3594cc27eb4d</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/72876af8-a89e-4ec9-950e-6291c7a10d79</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/cb173500-4d67-475a-88f8-91b731303f1b</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/35868143-c860-4403-989b-f06b3e57801a</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/9ce09470-d577-44ff-8f24-ca3ddd8160e8</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/bef30d8f-87bd-46ce-98bb-73a6510115fc</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/d22ed3a6-4ccb-42ef-b870-d6656a8aa797</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/bc54152a-a47f-405d-9862-0407f0e03227</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/8b53a35a-5926-4442-a778-c644ab834f7c</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/a286b5e9-042f-4fe3-b40a-83adbedce9a6</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/bed06f8c-641e-48a1-bf71-0f516a089fe3</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/a94442a0-7b33-4861-a079-72150483b547</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/a832cab0-0d5d-4c8a-ada2-b8793115fae3</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/2b4e38c5-342f-424f-bc19-93f68f09d963</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/968ba537-ee1b-422b-a27d-3fd9567f8cc4</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/4b233952-24b7-4e41-91b9-7a908753afbf</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/264ebbb5-2b4a-4c94-8e5f-4ac46b89e9ba</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/76cd6f23-fc0f-45eb-b2d1-c272ad540f30</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/b0df3496-be24-4568-8227-eb4962ddafde</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/eb93e6cd-e313-4b65-be86-1911e98adab7</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/4209cc72-b40f-4f26-962c-3a5f1579747a</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/683974e9-18be-4f23-9733-39ef9fdea9c7</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/38fbcf78-8192-4a12-84b8-ab8e35c4e3ba</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/f5e99d23-4790-4c1d-b670-e6b10cbc1804</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/eb02eea3-d592-4d14-92af-5238fab78a10</t>
+  </si>
+  <si>
+    <t>https://davesredistricting.org/join/9599c62a-f3b0-43b5-8404-9750a104aa1f</t>
+  </si>
+  <si>
+    <t>Only two districts</t>
+  </si>
+  <si>
+    <t>1. States with 3 or more congressional districts</t>
+  </si>
+  <si>
+    <t>2. States we have full composites for the period 2016–2020 (two P, two S, a G, and an AG)</t>
+  </si>
+  <si>
+    <t>3. States not using 2021 or later election data</t>
+  </si>
+  <si>
+    <t>31 states match these criteria</t>
+  </si>
+  <si>
+    <t>Criteria for study:</t>
   </si>
 </sst>
 </file>
@@ -892,11 +1043,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +1060,8 @@
     <col min="6" max="11" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="44" bestFit="1" customWidth="1"/>
-    <col min="14" max="20" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -990,6 +1142,9 @@
       <c r="K2" t="s">
         <v>6</v>
       </c>
+      <c r="N2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1048,6 +1203,9 @@
       <c r="K4" t="s">
         <v>6</v>
       </c>
+      <c r="N4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1083,6 +1241,9 @@
       <c r="K5" t="s">
         <v>6</v>
       </c>
+      <c r="N5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1118,6 +1279,9 @@
       <c r="M6" t="s">
         <v>144</v>
       </c>
+      <c r="N6" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1153,6 +1317,9 @@
       <c r="K7" t="s">
         <v>6</v>
       </c>
+      <c r="N7" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1194,6 +1361,9 @@
       <c r="M8" t="s">
         <v>132</v>
       </c>
+      <c r="N8" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1252,6 +1422,9 @@
       <c r="K10" t="s">
         <v>6</v>
       </c>
+      <c r="N10" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1287,6 +1460,9 @@
       <c r="K11" t="s">
         <v>6</v>
       </c>
+      <c r="N11" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1328,6 +1504,9 @@
       <c r="M12" t="s">
         <v>143</v>
       </c>
+      <c r="N12" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1363,6 +1542,15 @@
       <c r="K13" t="s">
         <v>6</v>
       </c>
+      <c r="L13" t="s">
+        <v>129</v>
+      </c>
+      <c r="M13" t="s">
+        <v>190</v>
+      </c>
+      <c r="N13" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1398,6 +1586,9 @@
       <c r="K14" t="s">
         <v>6</v>
       </c>
+      <c r="N14" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1433,6 +1624,9 @@
       <c r="K15" t="s">
         <v>23</v>
       </c>
+      <c r="N15" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1468,8 +1662,11 @@
       <c r="K16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1503,8 +1700,11 @@
       <c r="K17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1538,8 +1738,11 @@
       <c r="M18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1576,8 +1779,11 @@
       <c r="M19" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1614,8 +1820,11 @@
       <c r="M20" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1649,8 +1858,11 @@
       <c r="K21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1684,8 +1896,11 @@
       <c r="K22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1719,8 +1934,11 @@
       <c r="K23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1760,8 +1978,11 @@
       <c r="M24" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1801,8 +2022,11 @@
       <c r="M25" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1836,8 +2060,11 @@
       <c r="K26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1871,8 +2098,17 @@
       <c r="K27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>129</v>
+      </c>
+      <c r="M27" t="s">
+        <v>190</v>
+      </c>
+      <c r="N27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1912,8 +2148,11 @@
       <c r="M28" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1947,8 +2186,11 @@
       <c r="K29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1985,8 +2227,11 @@
       <c r="M30" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2023,8 +2268,11 @@
       <c r="M31" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2058,8 +2306,11 @@
       <c r="K32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2093,8 +2344,11 @@
       <c r="K33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2128,8 +2382,11 @@
       <c r="K34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2152,7 +2409,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2186,8 +2443,11 @@
       <c r="K36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -2221,8 +2481,11 @@
       <c r="K37" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2256,8 +2519,11 @@
       <c r="K38" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2291,8 +2557,11 @@
       <c r="K39" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -2326,8 +2595,17 @@
       <c r="K40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>129</v>
+      </c>
+      <c r="M40" t="s">
+        <v>190</v>
+      </c>
+      <c r="N40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -2361,8 +2639,11 @@
       <c r="K41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2385,7 +2666,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2425,8 +2706,11 @@
       <c r="M43" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2460,8 +2744,11 @@
       <c r="K44" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -2501,8 +2788,11 @@
       <c r="M45" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2525,7 +2815,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -2565,8 +2855,11 @@
       <c r="M47" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -2600,8 +2893,11 @@
       <c r="K48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -2629,8 +2925,11 @@
       <c r="M49" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -2664,8 +2963,11 @@
       <c r="K50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>73</v>
       </c>
@@ -2689,11 +2991,49 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:L1" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}"/>
+  <autoFilter ref="E1:L51" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T51">
     <sortCondition ref="D2:D51"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A724B9B-D38C-8844-9439-5CD76E5A9E7F}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Parked files not used
</commit_message>
<xml_diff>
--- a/data/Elections by State.xlsx
+++ b/data/Elections by State.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3745F743-3855-4C4A-A7C3-ADAF7DCA185C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7E644-7EF7-134B-A786-B00591C75B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="3420" windowWidth="27260" windowHeight="16940" activeTab="1" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
+    <workbookView xWindow="13320" yWindow="2520" windowWidth="27260" windowHeight="16940" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Elections by State" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="197">
   <si>
     <t>AL</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>Criteria for study:</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -718,11 +721,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,11 +1047,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1068,7 @@
     <col min="15" max="20" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -1107,8 +1111,11 @@
       <c r="N1" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1145,8 +1152,11 @@
       <c r="N2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1168,8 +1178,11 @@
       <c r="M3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1206,8 +1219,11 @@
       <c r="N4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1244,8 +1260,11 @@
       <c r="N5" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1282,8 +1301,11 @@
       <c r="N6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1320,8 +1342,11 @@
       <c r="N7" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1364,8 +1389,11 @@
       <c r="N8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1387,8 +1415,11 @@
       <c r="M9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1425,8 +1456,11 @@
       <c r="N10" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1463,8 +1497,11 @@
       <c r="N11" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1507,8 +1544,11 @@
       <c r="N12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1551,8 +1591,11 @@
       <c r="N13" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1589,8 +1632,11 @@
       <c r="N14" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1627,8 +1673,11 @@
       <c r="N15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1665,8 +1714,11 @@
       <c r="N16" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1703,8 +1755,11 @@
       <c r="N17" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1741,8 +1796,11 @@
       <c r="N18" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1782,8 +1840,11 @@
       <c r="N19" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1823,8 +1884,11 @@
       <c r="N20" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1861,8 +1925,11 @@
       <c r="N21" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1899,8 +1966,11 @@
       <c r="N22" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1937,8 +2007,11 @@
       <c r="N23" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1981,8 +2054,11 @@
       <c r="N24" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2025,8 +2101,11 @@
       <c r="N25" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2063,8 +2142,11 @@
       <c r="N26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2107,8 +2189,11 @@
       <c r="N27" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2151,8 +2236,11 @@
       <c r="N28" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2189,8 +2277,11 @@
       <c r="N29" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2230,8 +2321,11 @@
       <c r="N30" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2271,8 +2365,11 @@
       <c r="N31" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2309,8 +2406,11 @@
       <c r="N32" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2347,8 +2447,11 @@
       <c r="N33" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2385,8 +2488,11 @@
       <c r="N34" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2408,8 +2514,11 @@
       <c r="M35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2446,8 +2555,11 @@
       <c r="N36" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -2484,8 +2596,11 @@
       <c r="N37" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2522,8 +2637,11 @@
       <c r="N38" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2560,8 +2678,11 @@
       <c r="N39" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -2604,8 +2725,11 @@
       <c r="N40" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -2642,8 +2766,11 @@
       <c r="N41" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2665,8 +2792,11 @@
       <c r="M42" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2709,8 +2839,11 @@
       <c r="N43" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2747,8 +2880,11 @@
       <c r="N44" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -2791,8 +2927,11 @@
       <c r="N45" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2814,8 +2953,11 @@
       <c r="M46" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -2858,8 +3000,11 @@
       <c r="N47" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -2896,8 +3041,11 @@
       <c r="N48" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -2928,8 +3076,11 @@
       <c r="N49" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -2966,8 +3117,11 @@
       <c r="N50" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" s="4">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>73</v>
       </c>
@@ -3004,7 +3158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A724B9B-D38C-8844-9439-5CD76E5A9E7F}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>